<commit_message>
Actualizar tabla de trabajadores y roles
</commit_message>
<xml_diff>
--- a/TRABAJADORES PIN.xlsx
+++ b/TRABAJADORES PIN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ralvarez\proyecto_montaje\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB518FC-9456-405D-AAEF-F4A39EDDFFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9EB149-0005-43C5-9552-ABEFAE13DF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{E759CDCC-8EB3-44D5-B8BE-6A2BCEF6452E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E759CDCC-8EB3-44D5-B8BE-6A2BCEF6452E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
   <si>
     <t>JOSE ANGEL PALENCIA FRIAS</t>
   </si>
@@ -134,9 +134,6 @@
     <t>CALIDAD 1</t>
   </si>
   <si>
-    <t>CALIDAD 2</t>
-  </si>
-  <si>
     <t>RUBEN ALVAREZ FERNANDEZ</t>
   </si>
   <si>
@@ -207,6 +204,18 @@
   </si>
   <si>
     <t>RESERVA 21</t>
+  </si>
+  <si>
+    <t>ROL</t>
+  </si>
+  <si>
+    <t>jefe_obra</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>trabajador</t>
   </si>
 </sst>
 </file>
@@ -252,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -275,27 +284,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE9E105-9A06-4A43-A651-FA2558C5644C}">
-  <dimension ref="B1:E55"/>
+  <dimension ref="B1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P18:P19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,9 +648,11 @@
         <v>30</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
@@ -663,6 +664,9 @@
       <c r="D2" s="3">
         <v>9686</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -674,6 +678,9 @@
       <c r="D3" s="3">
         <v>5888</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -685,6 +692,9 @@
       <c r="D4" s="3">
         <v>1155</v>
       </c>
+      <c r="E4" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -696,6 +706,9 @@
       <c r="D5" s="3">
         <v>1384</v>
       </c>
+      <c r="E5" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
@@ -707,6 +720,9 @@
       <c r="D6" s="3">
         <v>1304</v>
       </c>
+      <c r="E6" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
@@ -718,6 +734,9 @@
       <c r="D7" s="3">
         <v>2296</v>
       </c>
+      <c r="E7" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -729,6 +748,9 @@
       <c r="D8" s="3">
         <v>2330</v>
       </c>
+      <c r="E8" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
@@ -740,6 +762,9 @@
       <c r="D9" s="3">
         <v>9334</v>
       </c>
+      <c r="E9" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -751,6 +776,9 @@
       <c r="D10" s="3">
         <v>6805</v>
       </c>
+      <c r="E10" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -762,6 +790,9 @@
       <c r="D11" s="3">
         <v>5287</v>
       </c>
+      <c r="E11" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
@@ -773,6 +804,9 @@
       <c r="D12" s="3">
         <v>7682</v>
       </c>
+      <c r="E12" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
@@ -784,6 +818,9 @@
       <c r="D13" s="3">
         <v>3084</v>
       </c>
+      <c r="E13" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
@@ -795,6 +832,9 @@
       <c r="D14" s="3">
         <v>3867</v>
       </c>
+      <c r="E14" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -806,6 +846,9 @@
       <c r="D15" s="3">
         <v>9229</v>
       </c>
+      <c r="E15" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
@@ -817,8 +860,11 @@
       <c r="D16" s="3">
         <v>1058</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
@@ -828,8 +874,11 @@
       <c r="D17" s="3">
         <v>1006</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
@@ -839,8 +888,11 @@
       <c r="D18" s="3">
         <v>6683</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
@@ -850,8 +902,11 @@
       <c r="D19" s="3">
         <v>3225</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
@@ -861,8 +916,11 @@
       <c r="D20" s="3">
         <v>2453</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
@@ -872,8 +930,11 @@
       <c r="D21" s="3">
         <v>5819</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
@@ -883,8 +944,11 @@
       <c r="D22" s="3">
         <v>4751</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
@@ -894,8 +958,11 @@
       <c r="D23" s="3">
         <v>9384</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
@@ -905,8 +972,11 @@
       <c r="D24" s="3">
         <v>9766</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
@@ -916,8 +986,11 @@
       <c r="D25" s="3">
         <v>9050</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
@@ -927,8 +1000,11 @@
       <c r="D26" s="3">
         <v>3037</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
@@ -938,8 +1014,11 @@
       <c r="D27" s="3">
         <v>1970</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
@@ -949,8 +1028,11 @@
       <c r="D28" s="3">
         <v>1158</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
@@ -960,8 +1042,11 @@
       <c r="D29" s="3">
         <v>6196</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>28</v>
       </c>
@@ -971,8 +1056,11 @@
       <c r="D30" s="3">
         <v>7957</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>31</v>
       </c>
@@ -982,8 +1070,11 @@
       <c r="D31" s="3">
         <v>9866</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>32</v>
       </c>
@@ -991,260 +1082,318 @@
         <v>31</v>
       </c>
       <c r="D32" s="3">
-        <v>3749</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+        <v>1029</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D33" s="3">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+        <v>4185</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="3">
         <v>34</v>
       </c>
-      <c r="C34" s="3">
-        <v>33</v>
-      </c>
       <c r="D34" s="3">
-        <v>4185</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+        <v>5718</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D35" s="3">
-        <v>5718</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+        <v>3424</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D36" s="3">
-        <v>3424</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+        <v>3396</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D37" s="3">
-        <v>3396</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+        <v>7135</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C38" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D38" s="3">
-        <v>7135</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+        <v>8874</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D39" s="3">
-        <v>8874</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+        <v>7820</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C40" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D40" s="3">
-        <v>7820</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+        <v>2222</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C41" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D41" s="3">
-        <v>2222</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+        <v>9517</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C42" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D42" s="3">
-        <v>9517</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+        <v>9021</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C43" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D43" s="3">
-        <v>9021</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+        <v>8853</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C44" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D44" s="3">
-        <v>8853</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+        <v>1903</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C45" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D45" s="3">
-        <v>1903</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+        <v>1980</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C46" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D46" s="3">
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+        <v>3343</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C47" s="3">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D47" s="3">
-        <v>3343</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+        <v>3434</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C48" s="3">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D48" s="3">
-        <v>3434</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+        <v>1954</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C49" s="3">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D49" s="3">
-        <v>1954</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+        <v>1187</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C50" s="3">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D50" s="3">
-        <v>1187</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+        <v>7368</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C51" s="3">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D51" s="3">
-        <v>7368</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+        <v>8371</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C52" s="3">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D52" s="3">
-        <v>8371</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+        <v>5983</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C53" s="3">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D53" s="3">
-        <v>5983</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+        <v>8120</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C54" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D54" s="3">
-        <v>8120</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B55" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C55" s="3">
-        <v>54</v>
-      </c>
-      <c r="D55" s="3">
         <v>6216</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>